<commit_message>
2nd test case added
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="27">
   <si>
     <t>Run</t>
   </si>
@@ -67,22 +67,40 @@
     <t>Naveen</t>
   </si>
   <si>
+    <t>chrome32</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>pqr@gmail.com</t>
+  </si>
+  <si>
+    <t>mnp@gmail.com</t>
+  </si>
+  <si>
+    <t>TestCase_2</t>
+  </si>
+  <si>
+    <t>firefox64</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>chrome32</t>
-  </si>
-  <si>
-    <t>ie64</t>
-  </si>
-  <si>
     <t>FAIL</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t/>
   </si>
 </sst>
 </file>
@@ -90,7 +108,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,8 +124,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -122,19 +148,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -163,22 +201,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
     <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="1" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
+    <xf applyFill="1" borderId="0" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="6" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="7" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyFill="1" borderId="0" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="7" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="7" fontId="2" numFmtId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -457,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,116 +514,215 @@
     <col min="3" max="3" customWidth="true" width="14.28515625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="4.42578125" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="53.85546875" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="5" t="s">
+      <c r="E2"/>
+      <c r="F2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="10" t="s">
         <v>7</v>
       </c>
+      <c r="I2"/>
+      <c r="J2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3"/>
-      <c r="F3" s="5" t="s">
+      <c r="C3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="10" t="s">
         <v>7</v>
       </c>
+      <c r="I3"/>
+      <c r="J3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="C4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="E4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="10" t="s">
         <v>7</v>
+      </c>
+      <c r="I4"/>
+      <c r="J4"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>1</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5"/>
+      <c r="F5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="10">
+        <v>123789</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>2</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="10">
+        <v>123789</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>3</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="10">
+        <v>123789</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="I5"/>
+    <hyperlink r:id="rId2" ref="I6"/>
+    <hyperlink r:id="rId3" ref="I7"/>
+  </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;10&amp;K000000Schlumberger-Private</oddFooter>
   </headerFooter>

</xml_diff>